<commit_message>
leichte Änderungen in der Klasse PUCalcItem vorgenommen, Doku weiter geschrieben, Projekt kurz vor Abschluss.
</commit_message>
<xml_diff>
--- a/Doku/PA_ProjektAnalyse_TestRapporte_Alain_Hoch.xlsx
+++ b/Doku/PA_ProjektAnalyse_TestRapporte_Alain_Hoch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blueofficech-my.sharepoint.com/personal/a_hoch_blue-office_ch/Documents/IPA/boProjektAnalyse/Doku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08473F61-8577-4109-B522-17E3DE25A8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{08473F61-8577-4109-B522-17E3DE25A8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D0EA769-8793-472A-A060-939754988300}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2E54DB87-C627-4EFD-8900-8829348B26E4}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{2E54DB87-C627-4EFD-8900-8829348B26E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -162,14 +162,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -202,7 +202,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -223,35 +223,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -280,128 +251,75 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -418,10 +336,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -726,465 +640,711 @@
   </sheetPr>
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="4" width="31.42578125" customWidth="1"/>
-    <col min="5" max="5" width="118.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="118.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="75.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="I2" s="14" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="12" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-    </row>
-    <row r="3" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+    </row>
+    <row r="3" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="5">
         <v>44965</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="13" t="s">
+      <c r="J3" s="3"/>
+      <c r="K3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-    </row>
-    <row r="4" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="1">
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+    </row>
+    <row r="4" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="6">
         <v>2</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="I4" s="14" t="s">
+      <c r="F4" s="8"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="12" t="s">
+      <c r="J4" s="10"/>
+      <c r="K4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-    </row>
-    <row r="5" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28">
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+    </row>
+    <row r="5" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="11">
         <v>2</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="5">
         <v>44965</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="I5" s="14" t="s">
+      <c r="F5" s="18"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="13" t="s">
+      <c r="J5" s="10"/>
+      <c r="K5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-    </row>
-    <row r="6" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="17"/>
-      <c r="I6" s="14" t="s">
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+    </row>
+    <row r="6" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="11"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="12" t="s">
+      <c r="J6" s="10"/>
+      <c r="K6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-    </row>
-    <row r="7" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+    </row>
+    <row r="7" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
         <v>3</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="5">
         <v>44965</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="4">
         <v>1</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="18"/>
-    </row>
-    <row r="8" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="19"/>
-    </row>
-    <row r="9" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
+      <c r="F7" s="20"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11">
         <v>4</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="5">
         <v>44965</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="6">
         <v>1</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="1">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="11"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="6">
         <v>2</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="F10" s="15"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
         <v>5</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="5">
         <v>44965</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="4">
         <v>1</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="18"/>
-    </row>
-    <row r="12" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="19"/>
-    </row>
-    <row r="13" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28">
+      <c r="F11" s="20"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="11">
         <v>6</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="5">
         <v>44965</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="6">
         <v>1</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="1">
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="11"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="6">
         <v>2</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="21"/>
-    </row>
-    <row r="15" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="F14" s="17"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+    </row>
+    <row r="15" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
         <v>7</v>
       </c>
-      <c r="B15" s="26">
+      <c r="B15" s="5">
         <v>44965</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="4">
         <v>1</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="18"/>
-    </row>
-    <row r="16" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="19"/>
-    </row>
-    <row r="17" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22">
+      <c r="F15" s="20"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+    </row>
+    <row r="16" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="11">
         <v>8</v>
       </c>
-      <c r="B17" s="26">
+      <c r="B17" s="5">
         <v>44965</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="12">
         <v>1</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-    </row>
-    <row r="19" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+    </row>
+    <row r="18" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="11"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
         <v>9</v>
       </c>
-      <c r="B19" s="26">
+      <c r="B19" s="5">
         <v>44965</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="4">
         <v>1</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="28">
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+    </row>
+    <row r="20" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="11">
         <v>10</v>
       </c>
-      <c r="B21" s="26">
+      <c r="B21" s="5">
         <v>44965</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="4">
         <v>1</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F21" s="24" t="s">
+      <c r="F21" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="25"/>
-    </row>
-    <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28">
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="11"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+    </row>
+    <row r="23" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="11">
         <v>11</v>
       </c>
-      <c r="B23" s="26">
+      <c r="B23" s="5">
         <v>44966</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="4">
         <v>1</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28">
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+    </row>
+    <row r="24" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="11"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="11">
         <v>12</v>
       </c>
-      <c r="B25" s="26">
+      <c r="B25" s="5">
         <v>44967</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="4">
         <v>1</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="16"/>
-    </row>
-    <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="17"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+    </row>
+    <row r="26" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="11"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="79">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
+  <mergeCells count="80">
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="K2:P2"/>
+    <mergeCell ref="K3:P3"/>
+    <mergeCell ref="K4:P4"/>
+    <mergeCell ref="K5:P5"/>
+    <mergeCell ref="K6:P6"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="E25:E26"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="B3:B4"/>
@@ -1201,52 +1361,27 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="K2:P2"/>
-    <mergeCell ref="K3:P3"/>
-    <mergeCell ref="K4:P4"/>
-    <mergeCell ref="K5:P5"/>
-    <mergeCell ref="K6:P6"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="33" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="47" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>